<commit_message>
more text while addition
</commit_message>
<xml_diff>
--- a/szablon.xlsx
+++ b/szablon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piotr\Desktop\mieszkania\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65CB45A-4295-4CB7-A69D-85685196D81F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E7887F-E5C3-4ACB-B7F6-D63BBD92EBFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -644,7 +644,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -763,141 +763,138 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1223,7 +1220,7 @@
   <dimension ref="A2:N75"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:N3"/>
+      <selection activeCell="K16" sqref="K16:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,14 +1230,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
       <c r="G2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1255,22 +1252,22 @@
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
@@ -1295,20 +1292,20 @@
       <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="55"/>
+      <c r="N5" s="55"/>
     </row>
     <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
@@ -1317,14 +1314,14 @@
       <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="38"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="81"/>
+      <c r="H6" s="55"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
@@ -1339,16 +1336,16 @@
       <c r="B7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="49" t="s">
+      <c r="D7" s="55"/>
+      <c r="E7" s="81" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
       <c r="I7" s="10" t="s">
         <v>0</v>
       </c>
@@ -1364,10 +1361,10 @@
       <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="51"/>
+      <c r="C8" s="37"/>
       <c r="D8" s="12">
         <v>230</v>
       </c>
@@ -1388,10 +1385,10 @@
       <c r="A9" s="7">
         <v>5</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="51"/>
+      <c r="C9" s="37"/>
       <c r="D9" s="12" t="s">
         <v>15</v>
       </c>
@@ -1410,11 +1407,11 @@
       <c r="A10" s="7">
         <v>6</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
@@ -1427,330 +1424,378 @@
       <c r="N10" s="9"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="77" t="s">
+      <c r="A11" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="57" t="s">
+      <c r="C11" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="61"/>
-      <c r="E11" s="57" t="s">
+      <c r="D11" s="59"/>
+      <c r="E11" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="61"/>
-      <c r="G11" s="57" t="s">
+      <c r="F11" s="59"/>
+      <c r="G11" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="61"/>
-      <c r="I11" s="79" t="s">
+      <c r="H11" s="59"/>
+      <c r="I11" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="61"/>
-      <c r="K11" s="57" t="s">
+      <c r="J11" s="59"/>
+      <c r="K11" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="L11" s="61"/>
-      <c r="M11" s="57" t="s">
+      <c r="L11" s="59"/>
+      <c r="M11" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="N11" s="61"/>
+      <c r="N11" s="59"/>
     </row>
     <row r="12" spans="1:14" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="78"/>
-      <c r="B12" s="58"/>
-      <c r="C12" s="56" t="s">
+      <c r="A12" s="57"/>
+      <c r="B12" s="84"/>
+      <c r="C12" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="53"/>
-      <c r="E12" s="56" t="s">
+      <c r="D12" s="62"/>
+      <c r="E12" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="53"/>
-      <c r="G12" s="56" t="s">
+      <c r="F12" s="62"/>
+      <c r="G12" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="53"/>
-      <c r="I12" s="52" t="s">
+      <c r="H12" s="62"/>
+      <c r="I12" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="53"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="81"/>
-      <c r="N12" s="82"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="61"/>
+      <c r="L12" s="62"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="64"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="15"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="55"/>
-      <c r="L13" s="48"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="40"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="65"/>
+      <c r="L13" s="44"/>
+      <c r="M13" s="42"/>
+      <c r="N13" s="41"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="15"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="55"/>
-      <c r="L14" s="48"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="40"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="65"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="42"/>
+      <c r="N14" s="41"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="55"/>
-      <c r="L15" s="48"/>
-      <c r="M15" s="80"/>
-      <c r="N15" s="40"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="41"/>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="55"/>
-      <c r="L16" s="48"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="40"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="65"/>
+      <c r="L16" s="44"/>
+      <c r="M16" s="42"/>
+      <c r="N16" s="41"/>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="55"/>
-      <c r="L17" s="48"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="40"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="65"/>
+      <c r="L17" s="44"/>
+      <c r="M17" s="42"/>
+      <c r="N17" s="41"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="55"/>
-      <c r="L18" s="48"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="65"/>
+      <c r="L18" s="44"/>
       <c r="M18" s="18"/>
       <c r="N18" s="19"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="48"/>
-      <c r="K19" s="55"/>
-      <c r="L19" s="48"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="65"/>
+      <c r="L19" s="44"/>
       <c r="M19" s="18"/>
       <c r="N19" s="19"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="15"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="54"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="55"/>
-      <c r="L20" s="48"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="65"/>
+      <c r="L20" s="44"/>
       <c r="M20" s="18"/>
       <c r="N20" s="19"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="65"/>
+      <c r="L21" s="44"/>
       <c r="M21" s="18"/>
       <c r="N21" s="19"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="65"/>
+      <c r="L22" s="44"/>
       <c r="M22" s="18"/>
       <c r="N22" s="19"/>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="15"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="48"/>
-      <c r="K23" s="55"/>
-      <c r="L23" s="48"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="65"/>
+      <c r="L23" s="44"/>
       <c r="M23" s="18"/>
       <c r="N23" s="19"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="15"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="48"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="65"/>
+      <c r="L24" s="44"/>
       <c r="M24" s="18"/>
       <c r="N24" s="19"/>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="36"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="36"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="65"/>
+      <c r="L25" s="44"/>
       <c r="M25" s="18"/>
       <c r="N25" s="19"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="15"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="48"/>
-      <c r="I26" s="54"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="47"/>
-      <c r="L26" s="48"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="65"/>
+      <c r="L26" s="44"/>
       <c r="M26" s="18"/>
       <c r="N26" s="19"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="15"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="36"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="65"/>
+      <c r="L27" s="44"/>
       <c r="M27" s="18"/>
       <c r="N27" s="19"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="15"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="36"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="36"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="65"/>
+      <c r="L28" s="44"/>
       <c r="M28" s="18"/>
       <c r="N28" s="19"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="15"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="36"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="36"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="65"/>
+      <c r="L29" s="44"/>
       <c r="M29" s="18"/>
       <c r="N29" s="19"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="15"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="14"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="44"/>
+      <c r="K30" s="65"/>
+      <c r="L30" s="44"/>
       <c r="M30" s="18"/>
       <c r="N30" s="19"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="44"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="65"/>
+      <c r="L31" s="44"/>
       <c r="M31" s="18"/>
       <c r="N31" s="19"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="44"/>
+      <c r="K32" s="65"/>
+      <c r="L32" s="44"/>
       <c r="M32" s="18"/>
       <c r="N32" s="19"/>
     </row>
@@ -1791,86 +1836,86 @@
       <c r="N35" s="19"/>
     </row>
     <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="41" t="s">
+      <c r="A36" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="42"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="42"/>
-      <c r="H36" s="42"/>
-      <c r="I36" s="42"/>
-      <c r="J36" s="42"/>
-      <c r="K36" s="42"/>
-      <c r="L36" s="43"/>
-      <c r="M36" s="39"/>
-      <c r="N36" s="40"/>
+      <c r="B36" s="74"/>
+      <c r="C36" s="74"/>
+      <c r="D36" s="74"/>
+      <c r="E36" s="74"/>
+      <c r="F36" s="74"/>
+      <c r="G36" s="74"/>
+      <c r="H36" s="74"/>
+      <c r="I36" s="74"/>
+      <c r="J36" s="74"/>
+      <c r="K36" s="74"/>
+      <c r="L36" s="75"/>
+      <c r="M36" s="42"/>
+      <c r="N36" s="41"/>
     </row>
     <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="44"/>
-      <c r="B37" s="45"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="45"/>
-      <c r="H37" s="45"/>
-      <c r="I37" s="45"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="46"/>
-      <c r="M37" s="39"/>
-      <c r="N37" s="40"/>
+      <c r="A37" s="77"/>
+      <c r="B37" s="78"/>
+      <c r="C37" s="78"/>
+      <c r="D37" s="78"/>
+      <c r="E37" s="78"/>
+      <c r="F37" s="78"/>
+      <c r="G37" s="78"/>
+      <c r="H37" s="78"/>
+      <c r="I37" s="78"/>
+      <c r="J37" s="78"/>
+      <c r="K37" s="78"/>
+      <c r="L37" s="79"/>
+      <c r="M37" s="42"/>
+      <c r="N37" s="41"/>
     </row>
     <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
-      <c r="B38" s="62"/>
-      <c r="C38" s="42"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="42"/>
-      <c r="F38" s="42"/>
-      <c r="G38" s="42"/>
-      <c r="H38" s="42"/>
-      <c r="I38" s="42"/>
-      <c r="J38" s="42"/>
-      <c r="K38" s="42"/>
-      <c r="L38" s="43"/>
-      <c r="M38" s="39"/>
-      <c r="N38" s="40"/>
+      <c r="B38" s="73"/>
+      <c r="C38" s="74"/>
+      <c r="D38" s="74"/>
+      <c r="E38" s="74"/>
+      <c r="F38" s="74"/>
+      <c r="G38" s="74"/>
+      <c r="H38" s="74"/>
+      <c r="I38" s="74"/>
+      <c r="J38" s="74"/>
+      <c r="K38" s="74"/>
+      <c r="L38" s="75"/>
+      <c r="M38" s="42"/>
+      <c r="N38" s="41"/>
     </row>
     <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="14"/>
-      <c r="B39" s="63"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
-      <c r="G39" s="38"/>
-      <c r="H39" s="38"/>
-      <c r="I39" s="38"/>
-      <c r="J39" s="38"/>
-      <c r="K39" s="38"/>
-      <c r="L39" s="40"/>
-      <c r="M39" s="39"/>
-      <c r="N39" s="40"/>
+      <c r="B39" s="76"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="55"/>
+      <c r="F39" s="55"/>
+      <c r="G39" s="55"/>
+      <c r="H39" s="55"/>
+      <c r="I39" s="55"/>
+      <c r="J39" s="55"/>
+      <c r="K39" s="55"/>
+      <c r="L39" s="41"/>
+      <c r="M39" s="42"/>
+      <c r="N39" s="41"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="14"/>
-      <c r="B40" s="44"/>
-      <c r="C40" s="45"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="45"/>
-      <c r="G40" s="45"/>
-      <c r="H40" s="45"/>
-      <c r="I40" s="45"/>
-      <c r="J40" s="45"/>
-      <c r="K40" s="45"/>
-      <c r="L40" s="46"/>
-      <c r="M40" s="80"/>
-      <c r="N40" s="40"/>
+      <c r="B40" s="77"/>
+      <c r="C40" s="78"/>
+      <c r="D40" s="78"/>
+      <c r="E40" s="78"/>
+      <c r="F40" s="78"/>
+      <c r="G40" s="78"/>
+      <c r="H40" s="78"/>
+      <c r="I40" s="78"/>
+      <c r="J40" s="78"/>
+      <c r="K40" s="78"/>
+      <c r="L40" s="79"/>
+      <c r="M40" s="40"/>
+      <c r="N40" s="41"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
@@ -1892,23 +1937,23 @@
       <c r="A42" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B42" s="65" t="s">
+      <c r="B42" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="51"/>
-      <c r="D42" s="64" t="s">
+      <c r="C42" s="37"/>
+      <c r="D42" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="E42" s="38"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="38"/>
-      <c r="H42" s="38"/>
-      <c r="I42" s="38"/>
-      <c r="J42" s="38"/>
-      <c r="K42" s="38"/>
-      <c r="L42" s="38"/>
-      <c r="M42" s="38"/>
-      <c r="N42" s="38"/>
+      <c r="E42" s="55"/>
+      <c r="F42" s="55"/>
+      <c r="G42" s="55"/>
+      <c r="H42" s="55"/>
+      <c r="I42" s="55"/>
+      <c r="J42" s="55"/>
+      <c r="K42" s="55"/>
+      <c r="L42" s="55"/>
+      <c r="M42" s="55"/>
+      <c r="N42" s="55"/>
     </row>
     <row r="43" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
@@ -1922,47 +1967,47 @@
       <c r="E43" s="22"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
-      <c r="H43" s="76" t="s">
+      <c r="H43" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="I43" s="38"/>
-      <c r="J43" s="38"/>
-      <c r="K43" s="38"/>
-      <c r="L43" s="38"/>
-      <c r="M43" s="38"/>
-      <c r="N43" s="38"/>
+      <c r="I43" s="55"/>
+      <c r="J43" s="55"/>
+      <c r="K43" s="55"/>
+      <c r="L43" s="55"/>
+      <c r="M43" s="55"/>
+      <c r="N43" s="55"/>
     </row>
     <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B44" s="74" t="s">
+      <c r="B44" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C44" s="51"/>
-      <c r="D44" s="51"/>
-      <c r="E44" s="51"/>
-      <c r="F44" s="51"/>
-      <c r="G44" s="51"/>
-      <c r="H44" s="51"/>
-      <c r="I44" s="51"/>
-      <c r="J44" s="51"/>
-      <c r="K44" s="51"/>
-      <c r="L44" s="51"/>
-      <c r="M44" s="51"/>
-      <c r="N44" s="51"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="37"/>
+      <c r="I44" s="37"/>
+      <c r="J44" s="37"/>
+      <c r="K44" s="37"/>
+      <c r="L44" s="37"/>
+      <c r="M44" s="37"/>
+      <c r="N44" s="37"/>
     </row>
     <row r="45" spans="1:14" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="83" t="s">
+      <c r="B45" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="84"/>
-      <c r="D45" s="84"/>
-      <c r="E45" s="84"/>
-      <c r="F45" s="84"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="39"/>
       <c r="G45" s="23"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -1973,34 +2018,34 @@
       <c r="N45" s="1"/>
     </row>
     <row r="46" spans="1:14" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="70" t="s">
+      <c r="A46" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B46" s="70" t="s">
+      <c r="B46" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="85" t="s">
+      <c r="C46" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="D46" s="86"/>
-      <c r="E46" s="86"/>
-      <c r="F46" s="86"/>
-      <c r="G46" s="86"/>
-      <c r="H46" s="86"/>
-      <c r="I46" s="86"/>
-      <c r="J46" s="86"/>
-      <c r="K46" s="86"/>
-      <c r="L46" s="87"/>
-      <c r="M46" s="68" t="s">
+      <c r="D46" s="47"/>
+      <c r="E46" s="47"/>
+      <c r="F46" s="47"/>
+      <c r="G46" s="47"/>
+      <c r="H46" s="47"/>
+      <c r="I46" s="47"/>
+      <c r="J46" s="47"/>
+      <c r="K46" s="47"/>
+      <c r="L46" s="48"/>
+      <c r="M46" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="N46" s="70" t="s">
+      <c r="N46" s="49" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="71"/>
-      <c r="B47" s="71"/>
+      <c r="A47" s="67"/>
+      <c r="B47" s="67"/>
       <c r="C47" s="24" t="s">
         <v>44</v>
       </c>
@@ -2031,12 +2076,12 @@
       <c r="L47" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="M47" s="69"/>
-      <c r="N47" s="69"/>
+      <c r="M47" s="50"/>
+      <c r="N47" s="50"/>
     </row>
     <row r="48" spans="1:14" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="69"/>
-      <c r="B48" s="69"/>
+      <c r="A48" s="50"/>
+      <c r="B48" s="50"/>
       <c r="C48" s="25" t="s">
         <v>54</v>
       </c>
@@ -2372,14 +2417,14 @@
       <c r="A67" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B67" s="74" t="s">
+      <c r="B67" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="C67" s="51"/>
-      <c r="D67" s="51"/>
-      <c r="E67" s="51"/>
-      <c r="F67" s="51"/>
-      <c r="G67" s="51"/>
+      <c r="C67" s="37"/>
+      <c r="D67" s="37"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="37"/>
+      <c r="G67" s="37"/>
       <c r="H67" s="35"/>
       <c r="I67" s="35"/>
       <c r="J67" s="35"/>
@@ -2390,11 +2435,11 @@
     </row>
     <row r="68" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="35"/>
-      <c r="B68" s="72" t="s">
+      <c r="B68" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="C68" s="38"/>
-      <c r="D68" s="38"/>
+      <c r="C68" s="55"/>
+      <c r="D68" s="55"/>
       <c r="E68" s="35"/>
       <c r="F68" s="35"/>
       <c r="G68" s="35"/>
@@ -2426,13 +2471,13 @@
       <c r="A70" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B70" s="65" t="s">
+      <c r="B70" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="C70" s="51"/>
-      <c r="D70" s="51"/>
-      <c r="E70" s="51"/>
-      <c r="F70" s="51"/>
+      <c r="C70" s="37"/>
+      <c r="D70" s="37"/>
+      <c r="E70" s="37"/>
+      <c r="F70" s="37"/>
       <c r="G70" s="20"/>
       <c r="H70" s="35"/>
       <c r="I70" s="35"/>
@@ -2444,48 +2489,48 @@
     </row>
     <row r="71" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
-      <c r="B71" s="67" t="s">
+      <c r="B71" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="C71" s="51"/>
-      <c r="D71" s="51"/>
-      <c r="E71" s="51"/>
-      <c r="F71" s="51"/>
-      <c r="G71" s="51"/>
-      <c r="H71" s="51"/>
-      <c r="I71" s="51"/>
-      <c r="J71" s="51"/>
-      <c r="K71" s="51"/>
-      <c r="L71" s="51"/>
-      <c r="M71" s="51"/>
-      <c r="N71" s="51"/>
+      <c r="C71" s="37"/>
+      <c r="D71" s="37"/>
+      <c r="E71" s="37"/>
+      <c r="F71" s="37"/>
+      <c r="G71" s="37"/>
+      <c r="H71" s="37"/>
+      <c r="I71" s="37"/>
+      <c r="J71" s="37"/>
+      <c r="K71" s="37"/>
+      <c r="L71" s="37"/>
+      <c r="M71" s="37"/>
+      <c r="N71" s="37"/>
     </row>
     <row r="72" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="35"/>
-      <c r="B72" s="67"/>
-      <c r="C72" s="51"/>
-      <c r="D72" s="51"/>
-      <c r="E72" s="51"/>
-      <c r="F72" s="51"/>
-      <c r="G72" s="51"/>
-      <c r="H72" s="51"/>
-      <c r="I72" s="51"/>
-      <c r="J72" s="51"/>
-      <c r="K72" s="51"/>
-      <c r="L72" s="51"/>
-      <c r="M72" s="51"/>
-      <c r="N72" s="51"/>
+      <c r="B72" s="52"/>
+      <c r="C72" s="37"/>
+      <c r="D72" s="37"/>
+      <c r="E72" s="37"/>
+      <c r="F72" s="37"/>
+      <c r="G72" s="37"/>
+      <c r="H72" s="37"/>
+      <c r="I72" s="37"/>
+      <c r="J72" s="37"/>
+      <c r="K72" s="37"/>
+      <c r="L72" s="37"/>
+      <c r="M72" s="37"/>
+      <c r="N72" s="37"/>
     </row>
     <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="66" t="s">
+      <c r="A73" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="B73" s="51"/>
-      <c r="C73" s="51"/>
-      <c r="D73" s="51"/>
-      <c r="E73" s="51"/>
-      <c r="F73" s="51"/>
-      <c r="G73" s="51"/>
+      <c r="B73" s="37"/>
+      <c r="C73" s="37"/>
+      <c r="D73" s="37"/>
+      <c r="E73" s="37"/>
+      <c r="F73" s="37"/>
+      <c r="G73" s="37"/>
       <c r="H73" s="35"/>
       <c r="I73" s="35"/>
       <c r="J73" s="35"/>
@@ -2495,15 +2540,15 @@
       <c r="N73" s="35"/>
     </row>
     <row r="74" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="66" t="s">
+      <c r="A74" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="B74" s="51"/>
-      <c r="C74" s="51"/>
-      <c r="D74" s="51"/>
-      <c r="E74" s="51"/>
-      <c r="F74" s="51"/>
-      <c r="G74" s="51"/>
+      <c r="B74" s="37"/>
+      <c r="C74" s="37"/>
+      <c r="D74" s="37"/>
+      <c r="E74" s="37"/>
+      <c r="F74" s="37"/>
+      <c r="G74" s="37"/>
       <c r="H74" s="35"/>
       <c r="I74" s="35"/>
       <c r="J74" s="35"/>
@@ -2529,22 +2574,112 @@
       <c r="N75" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="108">
-    <mergeCell ref="B67:G67"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="C46:L46"/>
-    <mergeCell ref="N46:N47"/>
+  <mergeCells count="153">
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="C5:N5"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="A36:L37"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="B38:L40"/>
+    <mergeCell ref="D42:N42"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="A74:G74"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="B72:N72"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="M46:M47"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="A73:G73"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="B70:F70"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="B44:N44"/>
     <mergeCell ref="M13:N13"/>
@@ -2569,75 +2704,30 @@
     <mergeCell ref="K23:L23"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B46:B48"/>
-    <mergeCell ref="A74:G74"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="B72:N72"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="M46:M47"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="A73:G73"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="B38:L40"/>
-    <mergeCell ref="D42:N42"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="C5:N5"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="A36:L37"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="B67:G67"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="C46:L46"/>
+    <mergeCell ref="N46:N47"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
   </mergeCells>
   <conditionalFormatting sqref="G47:G65">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
added validation. Stable version 1.0
</commit_message>
<xml_diff>
--- a/szablon.xlsx
+++ b/szablon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piotr\Desktop\mieszkania\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E7887F-E5C3-4ACB-B7F6-D63BBD92EBFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E739D23B-D6D4-453E-8D6D-82980D205E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
   <si>
     <t>1A</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>PROTOKÓŁ NR</t>
+  </si>
+  <si>
+    <t>gniazdko kuchnia</t>
   </si>
 </sst>
 </file>
@@ -763,138 +766,138 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1220,7 +1223,7 @@
   <dimension ref="A2:N75"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16:L16"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,14 +1233,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
       <c r="G2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1252,22 +1255,22 @@
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
@@ -1292,20 +1295,20 @@
       <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="72" t="s">
+      <c r="C5" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
-      <c r="M5" s="55"/>
-      <c r="N5" s="55"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
     </row>
     <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
@@ -1314,14 +1317,14 @@
       <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="81" t="s">
+      <c r="C6" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="81"/>
-      <c r="H6" s="55"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="41"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
@@ -1336,16 +1339,16 @@
       <c r="B7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="72" t="s">
+      <c r="C7" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="55"/>
-      <c r="E7" s="81" t="s">
+      <c r="D7" s="41"/>
+      <c r="E7" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
       <c r="I7" s="10" t="s">
         <v>0</v>
       </c>
@@ -1361,10 +1364,10 @@
       <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="37"/>
+      <c r="C8" s="52"/>
       <c r="D8" s="12">
         <v>230</v>
       </c>
@@ -1385,10 +1388,10 @@
       <c r="A9" s="7">
         <v>5</v>
       </c>
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="37"/>
+      <c r="C9" s="52"/>
       <c r="D9" s="12" t="s">
         <v>15</v>
       </c>
@@ -1407,11 +1410,11 @@
       <c r="A10" s="7">
         <v>6</v>
       </c>
-      <c r="B10" s="85" t="s">
+      <c r="B10" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
@@ -1424,378 +1427,380 @@
       <c r="N10" s="9"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="58" t="s">
+      <c r="C11" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="59"/>
-      <c r="E11" s="58" t="s">
+      <c r="D11" s="60"/>
+      <c r="E11" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="59"/>
-      <c r="G11" s="58" t="s">
+      <c r="F11" s="60"/>
+      <c r="G11" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="59"/>
-      <c r="I11" s="60" t="s">
+      <c r="H11" s="60"/>
+      <c r="I11" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="59"/>
-      <c r="K11" s="58" t="s">
+      <c r="J11" s="60"/>
+      <c r="K11" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="L11" s="59"/>
-      <c r="M11" s="58" t="s">
+      <c r="L11" s="60"/>
+      <c r="M11" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="N11" s="59"/>
+      <c r="N11" s="60"/>
     </row>
     <row r="12" spans="1:14" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="57"/>
-      <c r="B12" s="84"/>
-      <c r="C12" s="61" t="s">
+      <c r="A12" s="77"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="62"/>
-      <c r="E12" s="61" t="s">
+      <c r="D12" s="54"/>
+      <c r="E12" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="62"/>
-      <c r="G12" s="61" t="s">
+      <c r="F12" s="54"/>
+      <c r="G12" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="62"/>
-      <c r="I12" s="83" t="s">
+      <c r="H12" s="54"/>
+      <c r="I12" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="62"/>
-      <c r="K12" s="61"/>
-      <c r="L12" s="62"/>
-      <c r="M12" s="63"/>
-      <c r="N12" s="64"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="55"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="80"/>
+      <c r="N12" s="81"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="65"/>
-      <c r="L13" s="44"/>
+      <c r="B13" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="36"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="37"/>
       <c r="M13" s="42"/>
-      <c r="N13" s="41"/>
+      <c r="N13" s="43"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="15"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="44"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="37"/>
       <c r="M14" s="42"/>
-      <c r="N14" s="41"/>
+      <c r="N14" s="43"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="45"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="65"/>
-      <c r="L15" s="44"/>
-      <c r="M15" s="40"/>
-      <c r="N15" s="41"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="79"/>
+      <c r="N15" s="43"/>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="45"/>
-      <c r="J16" s="44"/>
-      <c r="K16" s="65"/>
-      <c r="L16" s="44"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="37"/>
       <c r="M16" s="42"/>
-      <c r="N16" s="41"/>
+      <c r="N16" s="43"/>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="44"/>
-      <c r="K17" s="65"/>
-      <c r="L17" s="44"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="37"/>
       <c r="M17" s="42"/>
-      <c r="N17" s="41"/>
+      <c r="N17" s="43"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="44"/>
-      <c r="K18" s="65"/>
-      <c r="L18" s="44"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="37"/>
       <c r="M18" s="18"/>
       <c r="N18" s="19"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="65"/>
-      <c r="L19" s="44"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="37"/>
       <c r="M19" s="18"/>
       <c r="N19" s="19"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="15"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="44"/>
-      <c r="K20" s="65"/>
-      <c r="L20" s="44"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="37"/>
       <c r="M20" s="18"/>
       <c r="N20" s="19"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="44"/>
-      <c r="K21" s="65"/>
-      <c r="L21" s="44"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="37"/>
       <c r="M21" s="18"/>
       <c r="N21" s="19"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="44"/>
-      <c r="K22" s="65"/>
-      <c r="L22" s="44"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="37"/>
       <c r="M22" s="18"/>
       <c r="N22" s="19"/>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="15"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="44"/>
-      <c r="K23" s="65"/>
-      <c r="L23" s="44"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="37"/>
       <c r="M23" s="18"/>
       <c r="N23" s="19"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="15"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="44"/>
-      <c r="K24" s="65"/>
-      <c r="L24" s="44"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="37"/>
       <c r="M24" s="18"/>
       <c r="N24" s="19"/>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="44"/>
-      <c r="K25" s="65"/>
-      <c r="L25" s="44"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="37"/>
       <c r="M25" s="18"/>
       <c r="N25" s="19"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="15"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="44"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="44"/>
-      <c r="K26" s="65"/>
-      <c r="L26" s="44"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="39"/>
+      <c r="L26" s="37"/>
       <c r="M26" s="18"/>
       <c r="N26" s="19"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="15"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="45"/>
-      <c r="J27" s="44"/>
-      <c r="K27" s="65"/>
-      <c r="L27" s="44"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="39"/>
+      <c r="L27" s="37"/>
       <c r="M27" s="18"/>
       <c r="N27" s="19"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="15"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="44"/>
-      <c r="K28" s="65"/>
-      <c r="L28" s="44"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="37"/>
       <c r="M28" s="18"/>
       <c r="N28" s="19"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="15"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="44"/>
-      <c r="K29" s="65"/>
-      <c r="L29" s="44"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="37"/>
       <c r="M29" s="18"/>
       <c r="N29" s="19"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="15"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="44"/>
-      <c r="K30" s="65"/>
-      <c r="L30" s="44"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="37"/>
       <c r="M30" s="18"/>
       <c r="N30" s="19"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="15"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="44"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="44"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="44"/>
-      <c r="K31" s="65"/>
-      <c r="L31" s="44"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="37"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="37"/>
       <c r="M31" s="18"/>
       <c r="N31" s="19"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="15"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="45"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="45"/>
-      <c r="H32" s="44"/>
-      <c r="I32" s="45"/>
-      <c r="J32" s="44"/>
-      <c r="K32" s="65"/>
-      <c r="L32" s="44"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="37"/>
       <c r="M32" s="18"/>
       <c r="N32" s="19"/>
     </row>
@@ -1836,86 +1841,86 @@
       <c r="N35" s="19"/>
     </row>
     <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="82" t="s">
+      <c r="A36" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="74"/>
-      <c r="C36" s="74"/>
-      <c r="D36" s="74"/>
-      <c r="E36" s="74"/>
-      <c r="F36" s="74"/>
-      <c r="G36" s="74"/>
-      <c r="H36" s="74"/>
-      <c r="I36" s="74"/>
-      <c r="J36" s="74"/>
-      <c r="K36" s="74"/>
-      <c r="L36" s="75"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="45"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="45"/>
+      <c r="K36" s="45"/>
+      <c r="L36" s="46"/>
       <c r="M36" s="42"/>
-      <c r="N36" s="41"/>
+      <c r="N36" s="43"/>
     </row>
     <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="77"/>
-      <c r="B37" s="78"/>
-      <c r="C37" s="78"/>
-      <c r="D37" s="78"/>
-      <c r="E37" s="78"/>
-      <c r="F37" s="78"/>
-      <c r="G37" s="78"/>
-      <c r="H37" s="78"/>
-      <c r="I37" s="78"/>
-      <c r="J37" s="78"/>
-      <c r="K37" s="78"/>
-      <c r="L37" s="79"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="48"/>
+      <c r="J37" s="48"/>
+      <c r="K37" s="48"/>
+      <c r="L37" s="49"/>
       <c r="M37" s="42"/>
-      <c r="N37" s="41"/>
+      <c r="N37" s="43"/>
     </row>
     <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
-      <c r="B38" s="73"/>
-      <c r="C38" s="74"/>
-      <c r="D38" s="74"/>
-      <c r="E38" s="74"/>
-      <c r="F38" s="74"/>
-      <c r="G38" s="74"/>
-      <c r="H38" s="74"/>
-      <c r="I38" s="74"/>
-      <c r="J38" s="74"/>
-      <c r="K38" s="74"/>
-      <c r="L38" s="75"/>
+      <c r="B38" s="61"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="45"/>
+      <c r="H38" s="45"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="45"/>
+      <c r="L38" s="46"/>
       <c r="M38" s="42"/>
-      <c r="N38" s="41"/>
+      <c r="N38" s="43"/>
     </row>
     <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="14"/>
-      <c r="B39" s="76"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="55"/>
-      <c r="E39" s="55"/>
-      <c r="F39" s="55"/>
-      <c r="G39" s="55"/>
-      <c r="H39" s="55"/>
-      <c r="I39" s="55"/>
-      <c r="J39" s="55"/>
-      <c r="K39" s="55"/>
-      <c r="L39" s="41"/>
+      <c r="B39" s="62"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="41"/>
+      <c r="G39" s="41"/>
+      <c r="H39" s="41"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="41"/>
+      <c r="K39" s="41"/>
+      <c r="L39" s="43"/>
       <c r="M39" s="42"/>
-      <c r="N39" s="41"/>
+      <c r="N39" s="43"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="14"/>
-      <c r="B40" s="77"/>
-      <c r="C40" s="78"/>
-      <c r="D40" s="78"/>
-      <c r="E40" s="78"/>
-      <c r="F40" s="78"/>
-      <c r="G40" s="78"/>
-      <c r="H40" s="78"/>
-      <c r="I40" s="78"/>
-      <c r="J40" s="78"/>
-      <c r="K40" s="78"/>
-      <c r="L40" s="79"/>
-      <c r="M40" s="40"/>
-      <c r="N40" s="41"/>
+      <c r="B40" s="47"/>
+      <c r="C40" s="48"/>
+      <c r="D40" s="48"/>
+      <c r="E40" s="48"/>
+      <c r="F40" s="48"/>
+      <c r="G40" s="48"/>
+      <c r="H40" s="48"/>
+      <c r="I40" s="48"/>
+      <c r="J40" s="48"/>
+      <c r="K40" s="48"/>
+      <c r="L40" s="49"/>
+      <c r="M40" s="79"/>
+      <c r="N40" s="43"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
@@ -1937,23 +1942,23 @@
       <c r="A42" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B42" s="71" t="s">
+      <c r="B42" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="37"/>
-      <c r="D42" s="80" t="s">
+      <c r="C42" s="52"/>
+      <c r="D42" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="E42" s="55"/>
-      <c r="F42" s="55"/>
-      <c r="G42" s="55"/>
-      <c r="H42" s="55"/>
-      <c r="I42" s="55"/>
-      <c r="J42" s="55"/>
-      <c r="K42" s="55"/>
-      <c r="L42" s="55"/>
-      <c r="M42" s="55"/>
-      <c r="N42" s="55"/>
+      <c r="E42" s="41"/>
+      <c r="F42" s="41"/>
+      <c r="G42" s="41"/>
+      <c r="H42" s="41"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="41"/>
+      <c r="K42" s="41"/>
+      <c r="L42" s="41"/>
+      <c r="M42" s="41"/>
+      <c r="N42" s="41"/>
     </row>
     <row r="43" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
@@ -1967,47 +1972,47 @@
       <c r="E43" s="22"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
-      <c r="H43" s="54" t="s">
+      <c r="H43" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="I43" s="55"/>
-      <c r="J43" s="55"/>
-      <c r="K43" s="55"/>
-      <c r="L43" s="55"/>
-      <c r="M43" s="55"/>
-      <c r="N43" s="55"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
+      <c r="K43" s="41"/>
+      <c r="L43" s="41"/>
+      <c r="M43" s="41"/>
+      <c r="N43" s="41"/>
     </row>
     <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B44" s="36" t="s">
+      <c r="B44" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="C44" s="37"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="37"/>
-      <c r="J44" s="37"/>
-      <c r="K44" s="37"/>
-      <c r="L44" s="37"/>
-      <c r="M44" s="37"/>
-      <c r="N44" s="37"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="52"/>
+      <c r="E44" s="52"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="52"/>
+      <c r="I44" s="52"/>
+      <c r="J44" s="52"/>
+      <c r="K44" s="52"/>
+      <c r="L44" s="52"/>
+      <c r="M44" s="52"/>
+      <c r="N44" s="52"/>
     </row>
     <row r="45" spans="1:14" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="38" t="s">
+      <c r="B45" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="39"/>
-      <c r="D45" s="39"/>
-      <c r="E45" s="39"/>
-      <c r="F45" s="39"/>
+      <c r="C45" s="83"/>
+      <c r="D45" s="83"/>
+      <c r="E45" s="83"/>
+      <c r="F45" s="83"/>
       <c r="G45" s="23"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -2018,34 +2023,34 @@
       <c r="N45" s="1"/>
     </row>
     <row r="46" spans="1:14" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="49" t="s">
+      <c r="A46" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="B46" s="49" t="s">
+      <c r="B46" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="46" t="s">
+      <c r="C46" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="D46" s="47"/>
-      <c r="E46" s="47"/>
-      <c r="F46" s="47"/>
-      <c r="G46" s="47"/>
-      <c r="H46" s="47"/>
-      <c r="I46" s="47"/>
-      <c r="J46" s="47"/>
-      <c r="K46" s="47"/>
-      <c r="L46" s="48"/>
-      <c r="M46" s="69" t="s">
+      <c r="D46" s="85"/>
+      <c r="E46" s="85"/>
+      <c r="F46" s="85"/>
+      <c r="G46" s="85"/>
+      <c r="H46" s="85"/>
+      <c r="I46" s="85"/>
+      <c r="J46" s="85"/>
+      <c r="K46" s="85"/>
+      <c r="L46" s="86"/>
+      <c r="M46" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="N46" s="49" t="s">
+      <c r="N46" s="69" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="67"/>
-      <c r="B47" s="67"/>
+      <c r="A47" s="70"/>
+      <c r="B47" s="70"/>
       <c r="C47" s="24" t="s">
         <v>44</v>
       </c>
@@ -2076,12 +2081,12 @@
       <c r="L47" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="M47" s="50"/>
-      <c r="N47" s="50"/>
+      <c r="M47" s="68"/>
+      <c r="N47" s="68"/>
     </row>
     <row r="48" spans="1:14" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="50"/>
-      <c r="B48" s="50"/>
+      <c r="A48" s="68"/>
+      <c r="B48" s="68"/>
       <c r="C48" s="25" t="s">
         <v>54</v>
       </c>
@@ -2417,14 +2422,14 @@
       <c r="A67" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B67" s="36" t="s">
+      <c r="B67" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="C67" s="37"/>
-      <c r="D67" s="37"/>
-      <c r="E67" s="37"/>
-      <c r="F67" s="37"/>
-      <c r="G67" s="37"/>
+      <c r="C67" s="52"/>
+      <c r="D67" s="52"/>
+      <c r="E67" s="52"/>
+      <c r="F67" s="52"/>
+      <c r="G67" s="52"/>
       <c r="H67" s="35"/>
       <c r="I67" s="35"/>
       <c r="J67" s="35"/>
@@ -2435,11 +2440,11 @@
     </row>
     <row r="68" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="35"/>
-      <c r="B68" s="70" t="s">
+      <c r="B68" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="C68" s="55"/>
-      <c r="D68" s="55"/>
+      <c r="C68" s="41"/>
+      <c r="D68" s="41"/>
       <c r="E68" s="35"/>
       <c r="F68" s="35"/>
       <c r="G68" s="35"/>
@@ -2471,13 +2476,13 @@
       <c r="A70" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B70" s="71" t="s">
+      <c r="B70" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="C70" s="37"/>
-      <c r="D70" s="37"/>
-      <c r="E70" s="37"/>
-      <c r="F70" s="37"/>
+      <c r="C70" s="52"/>
+      <c r="D70" s="52"/>
+      <c r="E70" s="52"/>
+      <c r="F70" s="52"/>
       <c r="G70" s="20"/>
       <c r="H70" s="35"/>
       <c r="I70" s="35"/>
@@ -2489,48 +2494,48 @@
     </row>
     <row r="71" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
-      <c r="B71" s="52" t="s">
+      <c r="B71" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="C71" s="37"/>
-      <c r="D71" s="37"/>
-      <c r="E71" s="37"/>
-      <c r="F71" s="37"/>
-      <c r="G71" s="37"/>
-      <c r="H71" s="37"/>
-      <c r="I71" s="37"/>
-      <c r="J71" s="37"/>
-      <c r="K71" s="37"/>
-      <c r="L71" s="37"/>
-      <c r="M71" s="37"/>
-      <c r="N71" s="37"/>
+      <c r="C71" s="52"/>
+      <c r="D71" s="52"/>
+      <c r="E71" s="52"/>
+      <c r="F71" s="52"/>
+      <c r="G71" s="52"/>
+      <c r="H71" s="52"/>
+      <c r="I71" s="52"/>
+      <c r="J71" s="52"/>
+      <c r="K71" s="52"/>
+      <c r="L71" s="52"/>
+      <c r="M71" s="52"/>
+      <c r="N71" s="52"/>
     </row>
     <row r="72" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="35"/>
-      <c r="B72" s="52"/>
-      <c r="C72" s="37"/>
-      <c r="D72" s="37"/>
-      <c r="E72" s="37"/>
-      <c r="F72" s="37"/>
-      <c r="G72" s="37"/>
-      <c r="H72" s="37"/>
-      <c r="I72" s="37"/>
-      <c r="J72" s="37"/>
-      <c r="K72" s="37"/>
-      <c r="L72" s="37"/>
-      <c r="M72" s="37"/>
-      <c r="N72" s="37"/>
+      <c r="B72" s="66"/>
+      <c r="C72" s="52"/>
+      <c r="D72" s="52"/>
+      <c r="E72" s="52"/>
+      <c r="F72" s="52"/>
+      <c r="G72" s="52"/>
+      <c r="H72" s="52"/>
+      <c r="I72" s="52"/>
+      <c r="J72" s="52"/>
+      <c r="K72" s="52"/>
+      <c r="L72" s="52"/>
+      <c r="M72" s="52"/>
+      <c r="N72" s="52"/>
     </row>
     <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="68" t="s">
+      <c r="A73" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="B73" s="37"/>
-      <c r="C73" s="37"/>
-      <c r="D73" s="37"/>
-      <c r="E73" s="37"/>
-      <c r="F73" s="37"/>
-      <c r="G73" s="37"/>
+      <c r="B73" s="52"/>
+      <c r="C73" s="52"/>
+      <c r="D73" s="52"/>
+      <c r="E73" s="52"/>
+      <c r="F73" s="52"/>
+      <c r="G73" s="52"/>
       <c r="H73" s="35"/>
       <c r="I73" s="35"/>
       <c r="J73" s="35"/>
@@ -2540,15 +2545,15 @@
       <c r="N73" s="35"/>
     </row>
     <row r="74" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="68" t="s">
+      <c r="A74" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="B74" s="37"/>
-      <c r="C74" s="37"/>
-      <c r="D74" s="37"/>
-      <c r="E74" s="37"/>
-      <c r="F74" s="37"/>
-      <c r="G74" s="37"/>
+      <c r="B74" s="52"/>
+      <c r="C74" s="52"/>
+      <c r="D74" s="52"/>
+      <c r="E74" s="52"/>
+      <c r="F74" s="52"/>
+      <c r="G74" s="52"/>
       <c r="H74" s="35"/>
       <c r="I74" s="35"/>
       <c r="J74" s="35"/>
@@ -2575,39 +2580,102 @@
     </row>
   </sheetData>
   <mergeCells count="153">
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="B67:G67"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="C46:L46"/>
+    <mergeCell ref="N46:N47"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="B44:N44"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="B71:N71"/>
+    <mergeCell ref="A3:N3"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="H43:N43"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="A74:G74"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="B72:N72"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="M46:M47"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="A73:G73"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="B38:L40"/>
+    <mergeCell ref="D42:N42"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
     <mergeCell ref="C5:N5"/>
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="A36:L37"/>
@@ -2632,102 +2700,39 @@
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="B38:L40"/>
-    <mergeCell ref="D42:N42"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="A74:G74"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="B72:N72"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="M46:M47"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="A73:G73"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="B44:N44"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="B71:N71"/>
-    <mergeCell ref="A3:N3"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="H43:N43"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="B67:G67"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="C46:L46"/>
-    <mergeCell ref="N46:N47"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
   </mergeCells>
   <conditionalFormatting sqref="G47:G65">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>